<commit_message>
summer update, primary results
</commit_message>
<xml_diff>
--- a/inputs/primary-results/raw/FED Results.xlsx
+++ b/inputs/primary-results/raw/FED Results.xlsx
@@ -26,10 +26,10 @@
     <x:t>State of Montana</x:t>
   </x:si>
   <x:si>
-    <x:t>Precincts 193 of 307 Reporting (Precincts Partially Reported: 100/307)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Downloaded at 6/8/2022 9:53:04 AM</x:t>
+    <x:t>Precincts 307 of 307 Reporting (Precincts Partially Reported: 0/307)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Downloaded at 7/19/2022 9:09:03 AM</x:t>
   </x:si>
   <x:si>
     <x:t>UNITED STATES REPRESENTATIVE
@@ -652,7 +652,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="61.480625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="59.350625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.990625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="20.030625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="12.460625" style="0" customWidth="1"/>
@@ -709,13 +709,13 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C8" s="1" t="n">
-        <x:v>983</x:v>
+        <x:v>988</x:v>
       </x:c>
       <x:c r="D8" s="1" t="n">
-        <x:v>218</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="E8" s="1" t="n">
-        <x:v>848</x:v>
+        <x:v>852</x:v>
       </x:c>
       <x:c r="F8" s="1" t="n">
         <x:v>42</x:v>
@@ -729,16 +729,16 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C9" s="1" t="n">
-        <x:v>353</x:v>
+        <x:v>359</x:v>
       </x:c>
       <x:c r="D9" s="1" t="n">
-        <x:v>140</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="E9" s="1" t="n">
-        <x:v>488</x:v>
+        <x:v>497</x:v>
       </x:c>
       <x:c r="F9" s="1" t="n">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="G9" s="1" t="n">
         <x:v>49</x:v>
@@ -749,19 +749,19 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C10" s="1" t="n">
-        <x:v>10335</x:v>
+        <x:v>10463</x:v>
       </x:c>
       <x:c r="D10" s="1" t="n">
-        <x:v>1970</x:v>
+        <x:v>2016</x:v>
       </x:c>
       <x:c r="E10" s="1" t="n">
-        <x:v>6814</x:v>
+        <x:v>6949</x:v>
       </x:c>
       <x:c r="F10" s="1" t="n">
-        <x:v>544</x:v>
+        <x:v>550</x:v>
       </x:c>
       <x:c r="G10" s="1" t="n">
-        <x:v>1969</x:v>
+        <x:v>1984</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
@@ -769,19 +769,19 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C11" s="1" t="n">
-        <x:v>5035</x:v>
+        <x:v>5062</x:v>
       </x:c>
       <x:c r="D11" s="1" t="n">
-        <x:v>1477</x:v>
+        <x:v>1490</x:v>
       </x:c>
       <x:c r="E11" s="1" t="n">
-        <x:v>5854</x:v>
+        <x:v>5891</x:v>
       </x:c>
       <x:c r="F11" s="1" t="n">
         <x:v>324</x:v>
       </x:c>
       <x:c r="G11" s="1" t="n">
-        <x:v>655</x:v>
+        <x:v>660</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
@@ -789,19 +789,19 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C12" s="1" t="n">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="D12" s="1" t="n">
-        <x:v>27</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E12" s="1" t="n">
-        <x:v>303</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="F12" s="1" t="n">
         <x:v>10</x:v>
       </x:c>
       <x:c r="G12" s="1" t="n">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
@@ -809,10 +809,10 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C13" s="1" t="n">
-        <x:v>318</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="D13" s="1" t="n">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="E13" s="1" t="n">
         <x:v>525</x:v>
@@ -829,19 +829,19 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C14" s="1" t="n">
-        <x:v>2525</x:v>
+        <x:v>2551</x:v>
       </x:c>
       <x:c r="D14" s="1" t="n">
-        <x:v>570</x:v>
+        <x:v>581</x:v>
       </x:c>
       <x:c r="E14" s="1" t="n">
-        <x:v>2245</x:v>
+        <x:v>2277</x:v>
       </x:c>
       <x:c r="F14" s="1" t="n">
         <x:v>124</x:v>
       </x:c>
       <x:c r="G14" s="1" t="n">
-        <x:v>262</x:v>
+        <x:v>265</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
@@ -849,19 +849,19 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>1617</x:v>
       </x:c>
       <x:c r="D15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>428</x:v>
       </x:c>
       <x:c r="E15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>2050</x:v>
       </x:c>
       <x:c r="F15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="G15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>167</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:7">
@@ -869,19 +869,19 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="C16" s="1" t="n">
-        <x:v>835</x:v>
+        <x:v>851</x:v>
       </x:c>
       <x:c r="D16" s="1" t="n">
-        <x:v>255</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="E16" s="1" t="n">
-        <x:v>1058</x:v>
+        <x:v>1073</x:v>
       </x:c>
       <x:c r="F16" s="1" t="n">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G16" s="1" t="n">
-        <x:v>69</x:v>
+        <x:v>72</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:7">
@@ -909,19 +909,19 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C18" s="1" t="n">
-        <x:v>3766</x:v>
+        <x:v>4122</x:v>
       </x:c>
       <x:c r="D18" s="1" t="n">
-        <x:v>1236</x:v>
+        <x:v>1337</x:v>
       </x:c>
       <x:c r="E18" s="1" t="n">
-        <x:v>5403</x:v>
+        <x:v>5899</x:v>
       </x:c>
       <x:c r="F18" s="1" t="n">
-        <x:v>231</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="G18" s="1" t="n">
-        <x:v>632</x:v>
+        <x:v>730</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:7">
@@ -935,13 +935,13 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="E19" s="1" t="n">
-        <x:v>198</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F19" s="1" t="n">
         <x:v>9</x:v>
       </x:c>
       <x:c r="G19" s="1" t="n">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:7">
@@ -969,19 +969,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C21" s="1" t="n">
-        <x:v>3676</x:v>
+        <x:v>3721</x:v>
       </x:c>
       <x:c r="D21" s="1" t="n">
-        <x:v>1086</x:v>
+        <x:v>1102</x:v>
       </x:c>
       <x:c r="E21" s="1" t="n">
-        <x:v>4960</x:v>
+        <x:v>5003</x:v>
       </x:c>
       <x:c r="F21" s="1" t="n">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="G21" s="1" t="n">
-        <x:v>549</x:v>
+        <x:v>554</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:7">
@@ -989,16 +989,16 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="C22" s="1" t="n">
-        <x:v>1770</x:v>
+        <x:v>1776</x:v>
       </x:c>
       <x:c r="D22" s="1" t="n">
-        <x:v>321</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="E22" s="1" t="n">
-        <x:v>1411</x:v>
+        <x:v>1427</x:v>
       </x:c>
       <x:c r="F22" s="1" t="n">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="G22" s="1" t="n">
         <x:v>97</x:v>
@@ -1009,19 +1009,19 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="C23" s="1" t="n">
-        <x:v>1004</x:v>
+        <x:v>1008</x:v>
       </x:c>
       <x:c r="D23" s="1" t="n">
-        <x:v>497</x:v>
+        <x:v>498</x:v>
       </x:c>
       <x:c r="E23" s="1" t="n">
-        <x:v>1468</x:v>
+        <x:v>1475</x:v>
       </x:c>
       <x:c r="F23" s="1" t="n">
         <x:v>76</x:v>
       </x:c>
       <x:c r="G23" s="1" t="n">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:7">
@@ -1029,19 +1029,19 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C24" s="1" t="n">
-        <x:v>31688</x:v>
+        <x:v>33927</x:v>
       </x:c>
       <x:c r="D24" s="1" t="n">
-        <x:v>8275</x:v>
+        <x:v>8915</x:v>
       </x:c>
       <x:c r="E24" s="1" t="n">
-        <x:v>32752</x:v>
+        <x:v>35601</x:v>
       </x:c>
       <x:c r="F24" s="1" t="n">
-        <x:v>1812</x:v>
+        <x:v>1953</x:v>
       </x:c>
       <x:c r="G24" s="1" t="n">
-        <x:v>4671</x:v>
+        <x:v>4973</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1064,7 +1064,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="61.480625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="59.350625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.990625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="16.600625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="16.330625" style="0" customWidth="1"/>
@@ -1113,7 +1113,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C8" s="1" t="n">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="D8" s="1" t="n">
         <x:v>300</x:v>
@@ -1127,13 +1127,13 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C9" s="1" t="n">
-        <x:v>441</x:v>
+        <x:v>448</x:v>
       </x:c>
       <x:c r="D9" s="1" t="n">
-        <x:v>1032</x:v>
+        <x:v>1070</x:v>
       </x:c>
       <x:c r="E9" s="1" t="n">
-        <x:v>100</x:v>
+        <x:v>104</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
@@ -1141,13 +1141,13 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C10" s="1" t="n">
-        <x:v>1439</x:v>
+        <x:v>1451</x:v>
       </x:c>
       <x:c r="D10" s="1" t="n">
-        <x:v>3562</x:v>
+        <x:v>3590</x:v>
       </x:c>
       <x:c r="E10" s="1" t="n">
-        <x:v>451</x:v>
+        <x:v>457</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
@@ -1155,13 +1155,13 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="C11" s="1" t="n">
-        <x:v>4605</x:v>
+        <x:v>4640</x:v>
       </x:c>
       <x:c r="D11" s="1" t="n">
-        <x:v>7738</x:v>
+        <x:v>7778</x:v>
       </x:c>
       <x:c r="E11" s="1" t="n">
-        <x:v>992</x:v>
+        <x:v>999</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
@@ -1169,13 +1169,13 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C12" s="1" t="n">
-        <x:v>451</x:v>
+        <x:v>503</x:v>
       </x:c>
       <x:c r="D12" s="1" t="n">
-        <x:v>425</x:v>
+        <x:v>474</x:v>
       </x:c>
       <x:c r="E12" s="1" t="n">
-        <x:v>301</x:v>
+        <x:v>321</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
@@ -1197,13 +1197,13 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="C14" s="1" t="n">
-        <x:v>636</x:v>
+        <x:v>654</x:v>
       </x:c>
       <x:c r="D14" s="1" t="n">
-        <x:v>1516</x:v>
+        <x:v>1533</x:v>
       </x:c>
       <x:c r="E14" s="1" t="n">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
@@ -1211,13 +1211,13 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="D15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>569</x:v>
       </x:c>
       <x:c r="E15" s="1" t="n">
-        <x:v>0</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
@@ -1225,10 +1225,10 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="C16" s="1" t="n">
-        <x:v>259</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="D16" s="1" t="n">
-        <x:v>451</x:v>
+        <x:v>466</x:v>
       </x:c>
       <x:c r="E16" s="1" t="n">
         <x:v>45</x:v>
@@ -1242,7 +1242,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="D17" s="1" t="n">
-        <x:v>115</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="E17" s="1" t="n">
         <x:v>7</x:v>
@@ -1253,13 +1253,13 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="C18" s="1" t="n">
-        <x:v>3408</x:v>
+        <x:v>3878</x:v>
       </x:c>
       <x:c r="D18" s="1" t="n">
-        <x:v>12819</x:v>
+        <x:v>14304</x:v>
       </x:c>
       <x:c r="E18" s="1" t="n">
-        <x:v>1531</x:v>
+        <x:v>1800</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:5">
@@ -1267,13 +1267,13 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C19" s="1" t="n">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="D19" s="1" t="n">
-        <x:v>29</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="E19" s="1" t="n">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
@@ -1295,13 +1295,13 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C21" s="1" t="n">
-        <x:v>697</x:v>
+        <x:v>703</x:v>
       </x:c>
       <x:c r="D21" s="1" t="n">
-        <x:v>2463</x:v>
+        <x:v>2473</x:v>
       </x:c>
       <x:c r="E21" s="1" t="n">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:5">
@@ -1309,13 +1309,13 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="C22" s="1" t="n">
-        <x:v>262</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="D22" s="1" t="n">
-        <x:v>629</x:v>
+        <x:v>633</x:v>
       </x:c>
       <x:c r="E22" s="1" t="n">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
@@ -1323,13 +1323,13 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="C23" s="1" t="n">
-        <x:v>1836</x:v>
+        <x:v>1841</x:v>
       </x:c>
       <x:c r="D23" s="1" t="n">
-        <x:v>3390</x:v>
+        <x:v>3409</x:v>
       </x:c>
       <x:c r="E23" s="1" t="n">
-        <x:v>363</x:v>
+        <x:v>364</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
@@ -1337,13 +1337,13 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C24" s="1" t="n">
-        <x:v>14440</x:v>
+        <x:v>15396</x:v>
       </x:c>
       <x:c r="D24" s="1" t="n">
-        <x:v>34853</x:v>
+        <x:v>37138</x:v>
       </x:c>
       <x:c r="E24" s="1" t="n">
-        <x:v>4316</x:v>
+        <x:v>4723</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1366,7 +1366,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="61.480625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="59.350625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="13.610625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="15.610625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="17.630625" style="0" customWidth="1"/>
@@ -1456,7 +1456,7 @@
         <x:v>91</x:v>
       </x:c>
       <x:c r="D10" s="1" t="n">
-        <x:v>1174</x:v>
+        <x:v>1176</x:v>
       </x:c>
       <x:c r="E10" s="1" t="n">
         <x:v>152</x:v>
@@ -1473,7 +1473,7 @@
         <x:v>123</x:v>
       </x:c>
       <x:c r="D11" s="1" t="n">
-        <x:v>1684</x:v>
+        <x:v>1685</x:v>
       </x:c>
       <x:c r="E11" s="1" t="n">
         <x:v>232</x:v>
@@ -1507,10 +1507,10 @@
         <x:v>765</x:v>
       </x:c>
       <x:c r="D13" s="1" t="n">
-        <x:v>9103</x:v>
+        <x:v>9124</x:v>
       </x:c>
       <x:c r="E13" s="1" t="n">
-        <x:v>1437</x:v>
+        <x:v>1438</x:v>
       </x:c>
       <x:c r="F13" s="1" t="n">
         <x:v>1194</x:v>
@@ -1521,7 +1521,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="C14" s="1" t="n">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="D14" s="1" t="n">
         <x:v>873</x:v>
@@ -1541,10 +1541,10 @@
         <x:v>120</x:v>
       </x:c>
       <x:c r="D15" s="1" t="n">
-        <x:v>1831</x:v>
+        <x:v>1835</x:v>
       </x:c>
       <x:c r="E15" s="1" t="n">
-        <x:v>324</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="F15" s="1" t="n">
         <x:v>125</x:v>
@@ -1575,7 +1575,7 @@
         <x:v>89</x:v>
       </x:c>
       <x:c r="D17" s="1" t="n">
-        <x:v>1554</x:v>
+        <x:v>1558</x:v>
       </x:c>
       <x:c r="E17" s="1" t="n">
         <x:v>223</x:v>
@@ -1606,16 +1606,16 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="C19" s="1" t="n">
-        <x:v>47</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="D19" s="1" t="n">
-        <x:v>1161</x:v>
+        <x:v>2486</x:v>
       </x:c>
       <x:c r="E19" s="1" t="n">
-        <x:v>124</x:v>
+        <x:v>259</x:v>
       </x:c>
       <x:c r="F19" s="1" t="n">
-        <x:v>56</x:v>
+        <x:v>142</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:6">
@@ -1657,16 +1657,16 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="C22" s="1" t="n">
-        <x:v>55</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="D22" s="1" t="n">
-        <x:v>992</x:v>
+        <x:v>1288</x:v>
       </x:c>
       <x:c r="E22" s="1" t="n">
-        <x:v>247</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="F22" s="1" t="n">
-        <x:v>65</x:v>
+        <x:v>96</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:6">
@@ -1674,16 +1674,16 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="C23" s="1" t="n">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D23" s="1" t="n">
-        <x:v>2030</x:v>
+        <x:v>2063</x:v>
       </x:c>
       <x:c r="E23" s="1" t="n">
-        <x:v>381</x:v>
+        <x:v>386</x:v>
       </x:c>
       <x:c r="F23" s="1" t="n">
-        <x:v>191</x:v>
+        <x:v>194</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:6">
@@ -1708,16 +1708,16 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="C25" s="1" t="n">
-        <x:v>433</x:v>
+        <x:v>583</x:v>
       </x:c>
       <x:c r="D25" s="1" t="n">
-        <x:v>5163</x:v>
+        <x:v>7187</x:v>
       </x:c>
       <x:c r="E25" s="1" t="n">
-        <x:v>1064</x:v>
+        <x:v>1388</x:v>
       </x:c>
       <x:c r="F25" s="1" t="n">
-        <x:v>519</x:v>
+        <x:v>663</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:6">
@@ -1765,7 +1765,7 @@
         <x:v>481</x:v>
       </x:c>
       <x:c r="E28" s="1" t="n">
-        <x:v>51</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F28" s="1" t="n">
         <x:v>29</x:v>
@@ -1793,16 +1793,16 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="C30" s="1" t="n">
-        <x:v>116</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="D30" s="1" t="n">
-        <x:v>2078</x:v>
+        <x:v>2096</x:v>
       </x:c>
       <x:c r="E30" s="1" t="n">
-        <x:v>298</x:v>
+        <x:v>301</x:v>
       </x:c>
       <x:c r="F30" s="1" t="n">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:6">
@@ -1847,10 +1847,10 @@
         <x:v>60</x:v>
       </x:c>
       <x:c r="D33" s="1" t="n">
-        <x:v>795</x:v>
+        <x:v>797</x:v>
       </x:c>
       <x:c r="E33" s="1" t="n">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="F33" s="1" t="n">
         <x:v>59</x:v>
@@ -1867,7 +1867,7 @@
         <x:v>613</x:v>
       </x:c>
       <x:c r="E34" s="1" t="n">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="F34" s="1" t="n">
         <x:v>30</x:v>
@@ -1895,10 +1895,10 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="C36" s="1" t="n">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="D36" s="1" t="n">
-        <x:v>1719</x:v>
+        <x:v>1734</x:v>
       </x:c>
       <x:c r="E36" s="1" t="n">
         <x:v>234</x:v>
@@ -1932,13 +1932,13 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="D38" s="1" t="n">
-        <x:v>1117</x:v>
+        <x:v>1121</x:v>
       </x:c>
       <x:c r="E38" s="1" t="n">
         <x:v>169</x:v>
       </x:c>
       <x:c r="F38" s="1" t="n">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:6">
@@ -1949,10 +1949,10 @@
         <x:v>63</x:v>
       </x:c>
       <x:c r="D39" s="1" t="n">
-        <x:v>719</x:v>
+        <x:v>720</x:v>
       </x:c>
       <x:c r="E39" s="1" t="n">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="F39" s="1" t="n">
         <x:v>68</x:v>
@@ -1966,7 +1966,7 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="D40" s="1" t="n">
-        <x:v>1798</x:v>
+        <x:v>1800</x:v>
       </x:c>
       <x:c r="E40" s="1" t="n">
         <x:v>250</x:v>
@@ -1980,16 +1980,16 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="C41" s="1" t="n">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D41" s="1" t="n">
-        <x:v>969</x:v>
+        <x:v>980</x:v>
       </x:c>
       <x:c r="E41" s="1" t="n">
         <x:v>148</x:v>
       </x:c>
       <x:c r="F41" s="1" t="n">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:6">
@@ -2017,13 +2017,13 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="D43" s="1" t="n">
-        <x:v>881</x:v>
+        <x:v>885</x:v>
       </x:c>
       <x:c r="E43" s="1" t="n">
         <x:v>122</x:v>
       </x:c>
       <x:c r="F43" s="1" t="n">
-        <x:v>61</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:6">
@@ -2099,16 +2099,16 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="C48" s="1" t="n">
-        <x:v>2251</x:v>
+        <x:v>2359</x:v>
       </x:c>
       <x:c r="D48" s="1" t="n">
-        <x:v>20395</x:v>
+        <x:v>21400</x:v>
       </x:c>
       <x:c r="E48" s="1" t="n">
-        <x:v>3797</x:v>
+        <x:v>3958</x:v>
       </x:c>
       <x:c r="F48" s="1" t="n">
-        <x:v>1479</x:v>
+        <x:v>1574</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:6">
@@ -2116,16 +2116,16 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C49" s="1" t="n">
-        <x:v>5373</x:v>
+        <x:v>5712</x:v>
       </x:c>
       <x:c r="D49" s="1" t="n">
-        <x:v>68681</x:v>
+        <x:v>73453</x:v>
       </x:c>
       <x:c r="E49" s="1" t="n">
-        <x:v>11216</x:v>
+        <x:v>11930</x:v>
       </x:c>
       <x:c r="F49" s="1" t="n">
-        <x:v>5552</x:v>
+        <x:v>5909</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2148,7 +2148,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="61.480625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="59.350625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="13.610625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="17.260625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="15.810625" style="0" customWidth="1"/>
@@ -2267,13 +2267,13 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="C13" s="1" t="n">
-        <x:v>1022</x:v>
+        <x:v>1023</x:v>
       </x:c>
       <x:c r="D13" s="1" t="n">
-        <x:v>1409</x:v>
+        <x:v>1410</x:v>
       </x:c>
       <x:c r="E13" s="1" t="n">
-        <x:v>2124</x:v>
+        <x:v>2125</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
@@ -2295,10 +2295,10 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="C15" s="1" t="n">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="D15" s="1" t="n">
-        <x:v>203</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="E15" s="1" t="n">
         <x:v>299</x:v>
@@ -2351,13 +2351,13 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="C19" s="1" t="n">
-        <x:v>42</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="D19" s="1" t="n">
-        <x:v>75</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="E19" s="1" t="n">
-        <x:v>151</x:v>
+        <x:v>343</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
@@ -2393,13 +2393,13 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="C22" s="1" t="n">
-        <x:v>217</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="D22" s="1" t="n">
-        <x:v>277</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="E22" s="1" t="n">
-        <x:v>345</x:v>
+        <x:v>411</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
@@ -2407,13 +2407,13 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="C23" s="1" t="n">
-        <x:v>208</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="D23" s="1" t="n">
-        <x:v>225</x:v>
+        <x:v>227</x:v>
       </x:c>
       <x:c r="E23" s="1" t="n">
-        <x:v>608</x:v>
+        <x:v>613</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
@@ -2435,13 +2435,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="C25" s="1" t="n">
-        <x:v>1185</x:v>
+        <x:v>1558</x:v>
       </x:c>
       <x:c r="D25" s="1" t="n">
-        <x:v>1876</x:v>
+        <x:v>2435</x:v>
       </x:c>
       <x:c r="E25" s="1" t="n">
-        <x:v>3689</x:v>
+        <x:v>4804</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
@@ -2483,7 +2483,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="E28" s="1" t="n">
-        <x:v>34</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:5">
@@ -2505,13 +2505,13 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="C30" s="1" t="n">
-        <x:v>436</x:v>
+        <x:v>441</x:v>
       </x:c>
       <x:c r="D30" s="1" t="n">
-        <x:v>229</x:v>
+        <x:v>232</x:v>
       </x:c>
       <x:c r="E30" s="1" t="n">
-        <x:v>1121</x:v>
+        <x:v>1127</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
@@ -2561,13 +2561,13 @@
         <x:v>61</x:v>
       </x:c>
       <x:c r="C34" s="1" t="n">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="D34" s="1" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="E34" s="1" t="n">
-        <x:v>7</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:5">
@@ -2592,10 +2592,10 @@
         <x:v>41</x:v>
       </x:c>
       <x:c r="D36" s="1" t="n">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E36" s="1" t="n">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:5">
@@ -2620,10 +2620,10 @@
         <x:v>49</x:v>
       </x:c>
       <x:c r="D38" s="1" t="n">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E38" s="1" t="n">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:5">
@@ -2645,7 +2645,7 @@
         <x:v>67</x:v>
       </x:c>
       <x:c r="C40" s="1" t="n">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="D40" s="1" t="n">
         <x:v>61</x:v>
@@ -2659,7 +2659,7 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="C41" s="1" t="n">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D41" s="1" t="n">
         <x:v>8</x:v>
@@ -2757,13 +2757,13 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="C48" s="1" t="n">
-        <x:v>1924</x:v>
+        <x:v>2045</x:v>
       </x:c>
       <x:c r="D48" s="1" t="n">
-        <x:v>1953</x:v>
+        <x:v>2032</x:v>
       </x:c>
       <x:c r="E48" s="1" t="n">
-        <x:v>8744</x:v>
+        <x:v>9167</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:5">
@@ -2771,13 +2771,13 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C49" s="1" t="n">
-        <x:v>6398</x:v>
+        <x:v>7029</x:v>
       </x:c>
       <x:c r="D49" s="1" t="n">
-        <x:v>7769</x:v>
+        <x:v>8586</x:v>
       </x:c>
       <x:c r="E49" s="1" t="n">
-        <x:v>20169</x:v>
+        <x:v>21983</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -2800,7 +2800,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="61.480625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="59.350625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="13.610625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="12.950625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="17.210625" style="0" customWidth="1"/>
@@ -2947,7 +2947,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="C15" s="1" t="n">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D15" s="1" t="n">
         <x:v>16</x:v>
@@ -3003,13 +3003,13 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="C19" s="1" t="n">
-        <x:v>14</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D19" s="1" t="n">
-        <x:v>11</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E19" s="1" t="n">
-        <x:v>2</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:5">
@@ -3045,13 +3045,13 @@
         <x:v>50</x:v>
       </x:c>
       <x:c r="C22" s="1" t="n">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D22" s="1" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E22" s="1" t="n">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:5">
@@ -3059,7 +3059,7 @@
         <x:v>51</x:v>
       </x:c>
       <x:c r="C23" s="1" t="n">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D23" s="1" t="n">
         <x:v>15</x:v>
@@ -3087,13 +3087,13 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="C25" s="1" t="n">
-        <x:v>116</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="D25" s="1" t="n">
-        <x:v>62</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E25" s="1" t="n">
-        <x:v>46</x:v>
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:5">
@@ -3157,13 +3157,13 @@
         <x:v>58</x:v>
       </x:c>
       <x:c r="C30" s="1" t="n">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D30" s="1" t="n">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E30" s="1" t="n">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">
@@ -3409,13 +3409,13 @@
         <x:v>75</x:v>
       </x:c>
       <x:c r="C48" s="1" t="n">
-        <x:v>423</x:v>
+        <x:v>453</x:v>
       </x:c>
       <x:c r="D48" s="1" t="n">
-        <x:v>265</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E48" s="1" t="n">
-        <x:v>249</x:v>
+        <x:v>271</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:5">
@@ -3423,13 +3423,13 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="C49" s="1" t="n">
-        <x:v>872</x:v>
+        <x:v>958</x:v>
       </x:c>
       <x:c r="D49" s="1" t="n">
-        <x:v>516</x:v>
+        <x:v>554</x:v>
       </x:c>
       <x:c r="E49" s="1" t="n">
-        <x:v>478</x:v>
+        <x:v>526</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>